<commit_message>
Migrate moutebank stub example to use api template framework. Add flag for mountebank api testing. Add create and delete stub functions in Before and After annotations.
</commit_message>
<xml_diff>
--- a/resources/template/apiTemplate.xlsx
+++ b/resources/template/apiTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kamal\auspost-javatestautomation\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willyeng/Documents/ampion/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F223B6AC-71EE-F74E-AC66-557B6CDD96F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12750" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Template</t>
   </si>
@@ -244,11 +245,23 @@
       }
     }</t>
   </si>
+  <si>
+    <t>mb</t>
+  </si>
+  <si>
+    <t>Create Stub</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>{"optionalField": true}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -682,23 +695,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -718,7 +731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="162" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -738,7 +751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -755,7 +768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -773,6 +786,26 @@
       </c>
       <c r="F4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>